<commit_message>
PROS-7988 PROS-7989 - CCRU - KPI templates update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - REG.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$59</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$59</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AL$59</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -285,7 +286,7 @@
     <t xml:space="preserve">Фанта Апельсин - 1л</t>
   </si>
   <si>
-    <t xml:space="preserve">5449000006271, 5449000006271</t>
+    <t xml:space="preserve">5449000006271, 5449000228963</t>
   </si>
   <si>
     <t xml:space="preserve">Sprite - 1L</t>
@@ -1091,7 +1092,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1173,6 +1174,10 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,48 +1321,48 @@
   </sheetPr>
   <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="AF1"/>
-      <selection pane="bottomLeft" activeCell="AJ60" activeCellId="0" sqref="AJ60"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="65.7692307692308"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="46.7044534412956"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="91.587044534413"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="82.1619433198381"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="92.336032388664"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="82.8016194331984"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.6032388663968"/>
@@ -1481,6 +1486,7 @@
       </c>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="n">
@@ -1543,6 +1549,7 @@
       <c r="AL2" s="13"/>
       <c r="AME2" s="15"/>
       <c r="AMF2" s="15"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
@@ -1604,6 +1611,7 @@
       </c>
       <c r="AL3" s="13"/>
       <c r="AMF3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
@@ -1667,6 +1675,7 @@
         <v>301</v>
       </c>
       <c r="AMF4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
@@ -1728,6 +1737,7 @@
       </c>
       <c r="AL5" s="13"/>
       <c r="AMF5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
@@ -1791,6 +1801,7 @@
         <v>310</v>
       </c>
       <c r="AMF6" s="0"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
@@ -1854,6 +1865,7 @@
         <v>310</v>
       </c>
       <c r="AMF7" s="0"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
@@ -1921,6 +1933,7 @@
         <v>300</v>
       </c>
       <c r="AMF8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="n">
@@ -2002,6 +2015,7 @@
         <v>1</v>
       </c>
       <c r="AMF9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="n">
@@ -2083,6 +2097,7 @@
         <v>1</v>
       </c>
       <c r="AMF10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="n">
@@ -2164,6 +2179,7 @@
         <v>1</v>
       </c>
       <c r="AMF11" s="0"/>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="n">
@@ -2199,7 +2215,7 @@
       <c r="M12" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="21" t="s">
         <v>77</v>
       </c>
       <c r="O12" s="13"/>
@@ -2245,6 +2261,7 @@
         <v>1</v>
       </c>
       <c r="AMF12" s="0"/>
+      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="n">
@@ -2326,6 +2343,7 @@
         <v>1</v>
       </c>
       <c r="AMF13" s="0"/>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="n">
@@ -2407,6 +2425,7 @@
         <v>1</v>
       </c>
       <c r="AMF14" s="0"/>
+      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
@@ -2488,6 +2507,7 @@
         <v>1</v>
       </c>
       <c r="AMF15" s="0"/>
+      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="n">
@@ -2508,7 +2528,7 @@
       <c r="F16" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="22" t="s">
         <v>88</v>
       </c>
       <c r="H16" s="8" t="s">
@@ -2567,6 +2587,7 @@
         <v>1</v>
       </c>
       <c r="AMF16" s="0"/>
+      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="n">
@@ -2587,7 +2608,7 @@
       <c r="F17" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="22" t="s">
         <v>92</v>
       </c>
       <c r="H17" s="8" t="s">
@@ -2648,6 +2669,7 @@
         <v>1</v>
       </c>
       <c r="AMF17" s="0"/>
+      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="n">
@@ -2668,7 +2690,7 @@
       <c r="F18" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="22" t="s">
         <v>95</v>
       </c>
       <c r="H18" s="8" t="s">
@@ -2729,6 +2751,7 @@
         <v>1</v>
       </c>
       <c r="AMF18" s="0"/>
+      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="n">
@@ -2810,6 +2833,7 @@
         <v>1</v>
       </c>
       <c r="AMF19" s="0"/>
+      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="n">
@@ -2891,6 +2915,7 @@
         <v>1</v>
       </c>
       <c r="AMF20" s="15"/>
+      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="n">
@@ -2908,10 +2933,10 @@
       <c r="E21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="24" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="8" t="s">
@@ -2923,10 +2948,10 @@
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="22" t="s">
+      <c r="M21" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="23" t="s">
+      <c r="N21" s="24" t="s">
         <v>105</v>
       </c>
       <c r="O21" s="13"/>
@@ -2972,6 +2997,7 @@
         <v>1</v>
       </c>
       <c r="AMF21" s="0"/>
+      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="n">
@@ -3039,6 +3065,7 @@
         <v>300</v>
       </c>
       <c r="AMF22" s="0"/>
+      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="n">
@@ -3120,6 +3147,7 @@
         <v>15</v>
       </c>
       <c r="AMF23" s="0"/>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="n">
@@ -3187,6 +3215,7 @@
         <v>300</v>
       </c>
       <c r="AMF24" s="0"/>
+      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="n">
@@ -3268,6 +3297,7 @@
         <v>17</v>
       </c>
       <c r="AMF25" s="0"/>
+      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="n">
@@ -3349,6 +3379,7 @@
         <v>17</v>
       </c>
       <c r="AMF26" s="0"/>
+      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="n">
@@ -3386,7 +3417,7 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
-      <c r="T27" s="24"/>
+      <c r="T27" s="25"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
@@ -3416,6 +3447,7 @@
         <v>300</v>
       </c>
       <c r="AMF27" s="0"/>
+      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="n">
@@ -3451,7 +3483,7 @@
       <c r="M28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="N28" s="25" t="s">
+      <c r="N28" s="26" t="s">
         <v>127</v>
       </c>
       <c r="O28" s="13"/>
@@ -3497,6 +3529,7 @@
         <v>20</v>
       </c>
       <c r="AMF28" s="15"/>
+      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="n">
@@ -3532,7 +3565,7 @@
       <c r="M29" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="N29" s="25" t="s">
+      <c r="N29" s="26" t="s">
         <v>130</v>
       </c>
       <c r="O29" s="13"/>
@@ -3578,6 +3611,7 @@
         <v>20</v>
       </c>
       <c r="AMF29" s="0"/>
+      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="n">
@@ -3645,6 +3679,7 @@
         <v>300</v>
       </c>
       <c r="AMF30" s="0"/>
+      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="n">
@@ -3726,6 +3761,7 @@
         <v>23</v>
       </c>
       <c r="AMF31" s="0"/>
+      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="n">
@@ -3807,6 +3843,7 @@
         <v>23</v>
       </c>
       <c r="AMF32" s="0"/>
+      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="n">
@@ -3888,6 +3925,7 @@
         <v>23</v>
       </c>
       <c r="AMF33" s="0"/>
+      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="n">
@@ -3969,6 +4007,7 @@
         <v>23</v>
       </c>
       <c r="AMF34" s="0"/>
+      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="n">
@@ -3986,7 +4025,7 @@
       <c r="E35" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="25" t="s">
         <v>146</v>
       </c>
       <c r="G35" s="13" t="s">
@@ -4001,7 +4040,7 @@
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
-      <c r="M35" s="24" t="s">
+      <c r="M35" s="25" t="s">
         <v>146</v>
       </c>
       <c r="N35" s="13" t="s">
@@ -4050,6 +4089,7 @@
         <v>23</v>
       </c>
       <c r="AMF35" s="0"/>
+      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="n">
@@ -4131,6 +4171,7 @@
         <v>23</v>
       </c>
       <c r="AMF36" s="0"/>
+      <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="n">
@@ -4197,7 +4238,7 @@
       <c r="AD37" s="11" t="n">
         <v>0.010007</v>
       </c>
-      <c r="AE37" s="24"/>
+      <c r="AE37" s="25"/>
       <c r="AF37" s="8"/>
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
@@ -4212,6 +4253,7 @@
         <v>23</v>
       </c>
       <c r="AMF37" s="15"/>
+      <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="n">
@@ -4292,6 +4334,7 @@
       <c r="AL38" s="8" t="n">
         <v>23</v>
       </c>
+      <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="n">
@@ -4334,7 +4377,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
-      <c r="U39" s="26"/>
+      <c r="U39" s="27"/>
       <c r="V39" s="8"/>
       <c r="W39" s="8" t="s">
         <v>162</v>
@@ -4363,9 +4406,10 @@
       <c r="AK39" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="AL39" s="24" t="n">
+      <c r="AL39" s="25" t="n">
         <v>303</v>
       </c>
+      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="n">
@@ -4414,7 +4458,7 @@
       </c>
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
-      <c r="U40" s="26"/>
+      <c r="U40" s="27"/>
       <c r="V40" s="8"/>
       <c r="W40" s="8" t="s">
         <v>162</v>
@@ -4442,6 +4486,7 @@
       <c r="AL40" s="8" t="n">
         <v>32</v>
       </c>
+      <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="n">
@@ -4484,7 +4529,7 @@
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
-      <c r="U41" s="26"/>
+      <c r="U41" s="27"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8" t="s">
         <v>162</v>
@@ -4514,6 +4559,7 @@
       <c r="AL41" s="8" t="n">
         <v>32</v>
       </c>
+      <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="n">
@@ -4560,7 +4606,7 @@
       </c>
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
-      <c r="U42" s="26"/>
+      <c r="U42" s="27"/>
       <c r="V42" s="8"/>
       <c r="W42" s="8" t="s">
         <v>162</v>
@@ -4590,6 +4636,7 @@
       <c r="AL42" s="8" t="n">
         <v>34</v>
       </c>
+      <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="n">
@@ -4617,7 +4664,7 @@
         <v>179</v>
       </c>
       <c r="I43" s="8"/>
-      <c r="J43" s="27"/>
+      <c r="J43" s="28"/>
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
       <c r="M43" s="8"/>
@@ -4662,6 +4709,7 @@
       <c r="AL43" s="8" t="n">
         <v>311</v>
       </c>
+      <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="n">
@@ -4744,6 +4792,7 @@
       <c r="AL44" s="8" t="n">
         <v>36</v>
       </c>
+      <c r="AMJ44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="n">
@@ -4826,6 +4875,7 @@
       <c r="AL45" s="8" t="n">
         <v>36</v>
       </c>
+      <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="n">
@@ -4900,6 +4950,7 @@
       <c r="AL46" s="8" t="n">
         <v>36</v>
       </c>
+      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="n">
@@ -4926,7 +4977,7 @@
       <c r="H47" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="I47" s="24"/>
+      <c r="I47" s="25"/>
       <c r="J47" s="10" t="n">
         <v>1</v>
       </c>
@@ -4980,6 +5031,7 @@
       <c r="AL47" s="8" t="n">
         <v>312</v>
       </c>
+      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="n">
@@ -5003,7 +5055,7 @@
       <c r="G48" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H48" s="28" t="s">
+      <c r="H48" s="29" t="s">
         <v>210</v>
       </c>
       <c r="I48" s="8"/>
@@ -5062,6 +5114,7 @@
       <c r="AL48" s="8" t="n">
         <v>312</v>
       </c>
+      <c r="AMJ48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="n">
@@ -5138,6 +5191,7 @@
       <c r="AL49" s="8" t="n">
         <v>312</v>
       </c>
+      <c r="AMJ49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="n">
@@ -5181,7 +5235,7 @@
       <c r="Q50" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R50" s="29" t="s">
+      <c r="R50" s="30" t="s">
         <v>220</v>
       </c>
       <c r="S50" s="8"/>
@@ -5220,6 +5274,7 @@
       <c r="AL50" s="8" t="n">
         <v>42</v>
       </c>
+      <c r="AMJ50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="n">
@@ -5294,6 +5349,7 @@
       <c r="AL51" s="8" t="n">
         <v>42</v>
       </c>
+      <c r="AMJ51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="n">
@@ -5312,7 +5368,7 @@
       <c r="F52" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="G52" s="30" t="s">
+      <c r="G52" s="31" t="s">
         <v>226</v>
       </c>
       <c r="H52" s="8" t="s">
@@ -5323,21 +5379,21 @@
         <v>4</v>
       </c>
       <c r="K52" s="10"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="30" t="s">
+      <c r="L52" s="32"/>
+      <c r="M52" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="N52" s="32" t="s">
+      <c r="N52" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32" t="s">
+      <c r="O52" s="33"/>
+      <c r="P52" s="33" t="s">
         <v>228</v>
       </c>
       <c r="Q52" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R52" s="29" t="s">
+      <c r="R52" s="30" t="s">
         <v>220</v>
       </c>
       <c r="S52" s="8"/>
@@ -5378,6 +5434,7 @@
       <c r="AL52" s="8" t="n">
         <v>45</v>
       </c>
+      <c r="AMJ52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="n">
@@ -5396,7 +5453,7 @@
       <c r="F53" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="G53" s="31" t="s">
         <v>232</v>
       </c>
       <c r="H53" s="8" t="s">
@@ -5408,20 +5465,20 @@
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
-      <c r="M53" s="30" t="s">
+      <c r="M53" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="N53" s="32" t="s">
+      <c r="N53" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32" t="s">
+      <c r="O53" s="33"/>
+      <c r="P53" s="33" t="s">
         <v>219</v>
       </c>
       <c r="Q53" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R53" s="29" t="s">
+      <c r="R53" s="30" t="s">
         <v>220</v>
       </c>
       <c r="S53" s="8"/>
@@ -5462,6 +5519,7 @@
       <c r="AL53" s="8" t="n">
         <v>45</v>
       </c>
+      <c r="AMJ53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="n">
@@ -5483,7 +5541,7 @@
       <c r="G54" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="H54" s="28" t="s">
+      <c r="H54" s="29" t="s">
         <v>237</v>
       </c>
       <c r="I54" s="8"/>
@@ -5503,7 +5561,7 @@
       <c r="Q54" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R54" s="29" t="s">
+      <c r="R54" s="30" t="s">
         <v>189</v>
       </c>
       <c r="S54" s="8"/>
@@ -5542,6 +5600,7 @@
       <c r="AL54" s="8" t="n">
         <v>42</v>
       </c>
+      <c r="AMJ54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="n">
@@ -5618,6 +5677,7 @@
       <c r="AL55" s="8" t="n">
         <v>312</v>
       </c>
+      <c r="AMJ55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="n">
@@ -5632,13 +5692,13 @@
       <c r="D56" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="E56" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F56" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="G56" s="22" t="s">
+      <c r="G56" s="23" t="s">
         <v>244</v>
       </c>
       <c r="H56" s="8" t="s">
@@ -5682,6 +5742,7 @@
         <v>54</v>
       </c>
       <c r="AL56" s="8"/>
+      <c r="AMJ56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="n">
@@ -5696,13 +5757,13 @@
       <c r="D57" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E57" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="G57" s="22" t="s">
+      <c r="G57" s="23" t="s">
         <v>250</v>
       </c>
       <c r="H57" s="8" t="s">
@@ -5750,6 +5811,7 @@
       </c>
       <c r="AK57" s="8"/>
       <c r="AL57" s="8"/>
+      <c r="AMJ57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="n">
@@ -5764,13 +5826,13 @@
       <c r="D58" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="E58" s="22" t="s">
+      <c r="E58" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="G58" s="22" t="s">
+      <c r="G58" s="23" t="s">
         <v>257</v>
       </c>
       <c r="H58" s="8" t="s">
@@ -5816,6 +5878,7 @@
       </c>
       <c r="AK58" s="8"/>
       <c r="AL58" s="8"/>
+      <c r="AMJ58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="n">
@@ -5830,13 +5893,13 @@
       <c r="D59" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E59" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="G59" s="22" t="s">
+      <c r="G59" s="23" t="s">
         <v>264</v>
       </c>
       <c r="H59" s="8" t="s">
@@ -5882,6 +5945,7 @@
       </c>
       <c r="AK59" s="8"/>
       <c r="AL59" s="8"/>
+      <c r="AMJ59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="n">
@@ -5896,11 +5960,11 @@
       <c r="D60" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22" t="s">
+      <c r="E60" s="23"/>
+      <c r="F60" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="G60" s="22" t="s">
+      <c r="G60" s="23" t="s">
         <v>267</v>
       </c>
       <c r="H60" s="8" t="s">
@@ -5913,7 +5977,7 @@
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
       <c r="M60" s="8"/>
-      <c r="N60" s="33"/>
+      <c r="N60" s="34"/>
       <c r="O60" s="8"/>
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
@@ -5931,7 +5995,7 @@
       <c r="AA60" s="8"/>
       <c r="AB60" s="8"/>
       <c r="AC60" s="8"/>
-      <c r="AD60" s="34"/>
+      <c r="AD60" s="35"/>
       <c r="AE60" s="8"/>
       <c r="AF60" s="8"/>
       <c r="AG60" s="8"/>

</xml_diff>